<commit_message>
created microscope slide with LED for pico testing
</commit_message>
<xml_diff>
--- a/meng-spad-quenching/active-quenching/pqar-wirebonded-rev1/bom/pqar-wirebonded-rev1-bom.xlsx
+++ b/meng-spad-quenching/active-quenching/pqar-wirebonded-rev1/bom/pqar-wirebonded-rev1-bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\Eagle-Public\meng-spad-quenching\active-quenching\pqar-wirebonded-rev1\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B4DC83-4FD4-49E8-B48D-D499E126F935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E413155E-3B81-41B3-82CA-155D47F8AF7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{07036CA5-4778-457A-9366-A0C8DBF17C4F}"/>
+    <workbookView minimized="1" xWindow="-28800" yWindow="5505" windowWidth="28800" windowHeight="12510" xr2:uid="{07036CA5-4778-457A-9366-A0C8DBF17C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -855,29 +855,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A217D37-6575-40C6-A08D-E660A087839F}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" customWidth="1"/>
-    <col min="5" max="5" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.90625" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -918,7 +918,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -945,7 +945,7 @@
       </c>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>2</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>A3+1</f>
         <v>3</v>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" ref="A5:A6" si="0">A4+1</f>
         <v>4</v>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f>A6+1</f>
         <v>6</v>
@@ -1087,7 +1087,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" ref="A8:A9" si="1">A7+1</f>
         <v>7</v>
@@ -1115,7 +1115,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1143,7 +1143,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f>A9+1</f>
         <v>9</v>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" ref="A11:A17" si="2">A10+1</f>
         <v>10</v>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <f>A17+1</f>
         <v>17</v>
@@ -1487,7 +1487,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f>A18+1</f>
         <v>18</v>
@@ -1515,7 +1515,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <f>A19+1</f>
         <v>19</v>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <f t="shared" ref="A21:A22" si="3">A20+1</f>
         <v>20</v>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f>A22+1</f>
         <v>22</v>
@@ -1627,7 +1627,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f>A23+1</f>
         <v>23</v>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" ref="A25:A27" si="4">A24+1</f>
         <v>24</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="4"/>
         <v>25</v>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="4"/>
         <v>26</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f>A27+1</f>
         <v>27</v>
@@ -1767,7 +1767,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <f>A28+1</f>
         <v>28</v>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <f>A29+1</f>
         <v>29</v>

</xml_diff>